<commit_message>
Added input file conventions to README
</commit_message>
<xml_diff>
--- a/examples/Versteeg/versteeg.xlsx
+++ b/examples/Versteeg/versteeg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebbuahin/Documents/Projects/HydroCouple/STMComponent/examples/Versteeg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74CEEDD-A7B1-6D47-A749-45EF8B436B8C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1C9806-2F74-654B-A942-33F48CDD489D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-123200" yWindow="-2540" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{FB56370F-BBCF-FD4C-B43E-F1DF9A3F1478}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="17540" activeTab="4" xr2:uid="{FB56370F-BBCF-FD4C-B43E-F1DF9A3F1478}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="5" r:id="rId1"/>
@@ -543,19 +543,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.87863341360000002</c:v>
+                  <c:v>0.94211</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73810372999999996</c:v>
+                  <c:v>0.80060092719999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58278136319999996</c:v>
+                  <c:v>0.62764557779999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41110937530000002</c:v>
+                  <c:v>0.41625552220000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2213665604</c:v>
+                  <c:v>0.1578900828</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,7 +923,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.8301214925453925E-2"/>
           <c:y val="9.5592783505154641E-2"/>
-          <c:w val="0.88875038558324537"/>
+          <c:w val="0.8506830679839984"/>
           <c:h val="0.76428461111651347"/>
         </c:manualLayout>
       </c:layout>
@@ -1454,8 +1454,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.8908361210484306E-2"/>
-              <c:y val="0.35270378145519005"/>
+              <c:x val="1.7444230525357096E-2"/>
+              <c:y val="0.38502696253877355"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1572,7 +1572,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D3148A60-AA72-E44E-BDF2-39CAEC396DD8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="165" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="171" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1583,7 +1583,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E79CC663-4DDC-C54D-8A1E-CA27BC037EB4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2047,7 +2047,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2092,7 +2092,7 @@
         <v>0.94211</v>
       </c>
       <c r="E2">
-        <v>0.87863341360000002</v>
+        <v>0.94211</v>
       </c>
       <c r="J2" s="5">
         <v>6.9444444439999999E-4</v>
@@ -2113,13 +2113,13 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.87863341360000002</v>
+        <v>0.94211</v>
       </c>
       <c r="Q2">
         <v>1</v>
       </c>
       <c r="R2">
-        <v>0.80836857179999999</v>
+        <v>0.87135546360000005</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -2137,7 +2137,7 @@
         <v>0.80060092719999998</v>
       </c>
       <c r="E3">
-        <v>0.73810372999999996</v>
+        <v>0.80060092719999998</v>
       </c>
       <c r="J3" s="5">
         <v>6.9444444439999999E-4</v>
@@ -2158,13 +2158,13 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.73810372999999996</v>
+        <v>0.80060092719999998</v>
       </c>
       <c r="Q3">
-        <v>0.80836857179999999</v>
+        <v>0.87135546360000005</v>
       </c>
       <c r="R3">
-        <v>0.66044254660000001</v>
+        <v>0.71412325249999997</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -2182,7 +2182,7 @@
         <v>0.62764557779999997</v>
       </c>
       <c r="E4">
-        <v>0.58278136319999996</v>
+        <v>0.62764557779999997</v>
       </c>
       <c r="J4" s="5">
         <v>6.9444444439999999E-4</v>
@@ -2203,13 +2203,13 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.58278136319999996</v>
+        <v>0.62764557779999997</v>
       </c>
       <c r="Q4">
-        <v>0.66044254660000001</v>
+        <v>0.71412325249999997</v>
       </c>
       <c r="R4">
-        <v>0.49694536919999999</v>
+        <v>0.52195055000000001</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -2227,7 +2227,7 @@
         <v>0.41625552220000001</v>
       </c>
       <c r="E5">
-        <v>0.41110937530000002</v>
+        <v>0.41625552220000001</v>
       </c>
       <c r="J5" s="5">
         <v>6.9444444439999999E-4</v>
@@ -2248,13 +2248,13 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.41110937530000002</v>
+        <v>0.41625552220000001</v>
       </c>
       <c r="Q5">
-        <v>0.49694536919999999</v>
+        <v>0.52195055000000001</v>
       </c>
       <c r="R5">
-        <v>0.31623796790000003</v>
+        <v>0.2870728025</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -2272,7 +2272,7 @@
         <v>0.1578900828</v>
       </c>
       <c r="E6">
-        <v>0.2213665604</v>
+        <v>0.1578900828</v>
       </c>
       <c r="J6" s="5">
         <v>6.9444444439999999E-4</v>
@@ -2293,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.2213665604</v>
+        <v>0.1578900828</v>
       </c>
       <c r="Q6">
-        <v>0.31623796790000003</v>
+        <v>0.2870728025</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2352,82 +2352,92 @@
       <c r="E16" s="2"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="E17" s="2"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="E18" s="2"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="E19" s="2"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="E20" s="2"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="E21" s="2"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="E22" s="2"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="E23" s="2"/>
       <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="E24" s="2"/>
       <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="O24">
+        <v>2.7489003276302002E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="E25" s="2"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="E26" s="2"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="E27" s="2"/>
       <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="O27">
+        <f>O24*2</f>
+        <v>5.4978006552604004E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="E28" s="2"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="E29" s="2"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="E30" s="2"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="E31" s="2"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="E32" s="2"/>
       <c r="J32" s="5"/>
@@ -2490,7 +2500,7 @@
   <dimension ref="A1:U101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added FileIO, Boundary Conditions, and CLI interface
</commit_message>
<xml_diff>
--- a/examples/Versteeg/versteeg.xlsx
+++ b/examples/Versteeg/versteeg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebbuahin/Documents/Projects/HydroCouple/STMComponent/examples/Versteeg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EA6A32-DFA8-F342-8000-300C8D441E6F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475F168-14C6-0241-BAA2-4EB135DC13CF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-128000" yWindow="-3140" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{FB56370F-BBCF-FD4C-B43E-F1DF9A3F1478}"/>
+    <workbookView xWindow="-123200" yWindow="-2540" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{FB56370F-BBCF-FD4C-B43E-F1DF9A3F1478}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="5" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="Profile_Case_2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="lookuptest">Case_2!$K$2:$O$6</definedName>
+    <definedName name="lookuptest">Case_2!$K$2:$P$6</definedName>
   </definedNames>
-  <calcPr calcId="171027" iterate="1" iterateCount="10000"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -993,15 +993,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
@@ -1019,26 +1010,86 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Case_2!$A$2:$A$42</c:f>
+              <c:f>Case_2!$N$2:$N$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="18">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1046,26 +1097,86 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Case_2!$B$2:$B$42</c:f>
+              <c:f>Case_2!$O$2:$O$29</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>0.99999999999099054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99999999995164646</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.99999999984469812</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>0.99999999955398244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99999999876373513</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99999999661562011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99999999077643831</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.99999997490389636</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>0.99999993175785418</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99999981447475172</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999949566622537</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99999862905480152</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.99999627336071584</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
+                  <c:v>0.99998986992028915</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99997246356453784</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99992514818399925</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99979653164487448</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.99944691564373245</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="18">
+                  <c:v>0.99849656082088944</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99591322857536713</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98889100347549141</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.96980261659115019</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.91791500138884918</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>0.77686983986236013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.39346934029283109</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1324,6 +1435,187 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8505-0D4A-B4FE-EEC3AD91931E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>STM Hybrid Higher Res</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Case_2!$N$2:$N$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Case_2!$R$2:$R$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.99999921300000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99999762459999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99999500959999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9999905925</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99998332729999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99997106879999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99995086089999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99991685939999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99986064330000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99976632450000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99960997429999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99934825940000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99891355479999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99818712129999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9969788571</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99496199139999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99160437739999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98600369290000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.97667478569999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96112010550000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.93520302609999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.89199979250000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.82000285689999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.69999979629999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.50000154299999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2BE5-1847-9DDC-307A21FE5775}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1448,6 +1740,7 @@
         <c:axId val="750468240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1566,8 +1859,8 @@
           <c:yMode val="edge"/>
           <c:x val="8.5752920589028683E-2"/>
           <c:y val="0.93766924212314895"/>
-          <c:w val="0.89228646326870797"/>
-          <c:h val="4.1443331522142211E-2"/>
+          <c:w val="0.80397195871539817"/>
+          <c:h val="4.1421299610275991E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1621,7 +1914,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D3148A60-AA72-E44E-BDF2-39CAEC396DD8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="165" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2093,10 +2386,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90045F8F-433E-F54C-8549-41D6119563B9}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2434,37 +2727,41 @@
       <c r="E16" s="2"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="E17" s="2"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="E18" s="2"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="E19" s="2"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="E20" s="2"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="E21" s="2"/>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="V21">
+        <f>0.1*0.1</f>
+        <v>1.0000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="E22" s="2"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="E23" s="2"/>
       <c r="J23" s="5"/>
@@ -2472,7 +2769,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="E24" s="2"/>
       <c r="J24" s="5"/>
@@ -2480,17 +2777,17 @@
         <v>2.7489003276302002E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="E25" s="2"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="E26" s="2"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="E27" s="2"/>
       <c r="J27" s="5"/>
@@ -2499,27 +2796,27 @@
         <v>5.4978006552604004E-4</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="E28" s="2"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="E29" s="2"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="E30" s="2"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="E31" s="2"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="E32" s="2"/>
       <c r="J32" s="5"/>
@@ -2579,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFF3520-1FA5-EC40-AAF0-84D17460CE68}">
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:V101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2594,7 +2891,7 @@
     <col min="8" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2614,7 +2911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -2644,25 +2941,29 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.1</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
+        <v>0.02</v>
+      </c>
+      <c r="O2" s="2">
+        <f>(((EXP(2.5*N2/0.1) - 1)/(EXP(2.5*1/0.1) - 1)) *-1) +1</f>
+        <v>0.99999999999099054</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>1.0356304119999999</v>
-      </c>
-      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0.99999921300000005</v>
+      </c>
+      <c r="S2" s="5">
         <v>1</v>
       </c>
-      <c r="S2">
-        <v>0.95249266860000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T2">
+        <v>0.99999841879999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.3</v>
       </c>
@@ -2692,26 +2993,30 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0.3</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0.86935492540000003</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0.95249266860000004</v>
-      </c>
-      <c r="S3">
-        <v>1.0633431090000001</v>
-      </c>
-      <c r="U3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0.06</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O25" si="1">(((EXP(2.5*N3/0.1) - 1)/(EXP(2.5*1/0.1) - 1)) *-1) +1</f>
+        <v>0.99999999995164646</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.99999762459999997</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0.99999841879999996</v>
+      </c>
+      <c r="T3">
+        <v>0.99999631710000003</v>
+      </c>
+      <c r="V3" s="4"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -2741,26 +3046,30 @@
         <v>2</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>1.2573312919999999</v>
-      </c>
-      <c r="R4" s="5">
-        <v>1.0633431090000001</v>
-      </c>
-      <c r="S4">
-        <v>0.80469208209999998</v>
-      </c>
-      <c r="U4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999999984469812</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0.99999500959999998</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.99999631710000003</v>
+      </c>
+      <c r="T4">
+        <v>0.99999280099999999</v>
+      </c>
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.7</v>
       </c>
@@ -2790,26 +3099,30 @@
         <v>3</v>
       </c>
       <c r="N5">
-        <v>0.7</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0.35205287270000002</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0.80469208209999998</v>
-      </c>
-      <c r="S5">
-        <v>1.408211144</v>
-      </c>
-      <c r="U5" s="4"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999999955398244</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0.9999905925</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0.99999280099999999</v>
+      </c>
+      <c r="T5">
+        <v>0.99998695989999997</v>
+      </c>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.9</v>
       </c>
@@ -2839,26 +3152,30 @@
         <v>4</v>
       </c>
       <c r="N6">
-        <v>0.9</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>2.4643694150000002</v>
-      </c>
-      <c r="R6" s="5">
-        <v>1.408211144</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0.18</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999999876373513</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.99998332729999995</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.99998695989999997</v>
+      </c>
+      <c r="T6">
+        <v>0.99997719799999996</v>
+      </c>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -2877,374 +3194,961 @@
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K7" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>0.22</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999999661562011</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0.99997106879999997</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0.99997719799999996</v>
+      </c>
+      <c r="T7">
+        <v>0.99996096489999997</v>
+      </c>
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8" s="2"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K8" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>0.26</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999999077643831</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0.99995086089999996</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0.99996096489999997</v>
+      </c>
+      <c r="T8">
+        <v>0.99993386009999996</v>
+      </c>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9" s="2"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K9" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>0.3</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999997490389636</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0.99991685939999997</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0.99993386009999996</v>
+      </c>
+      <c r="T9">
+        <v>0.9998887514</v>
+      </c>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10" s="2"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K10" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>0.34</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999993175785418</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0.99986064330000002</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.9998887514</v>
+      </c>
+      <c r="T10">
+        <v>0.99981348390000002</v>
+      </c>
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11" s="2"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K11" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>0.38</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999981447475172</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0.99976632450000003</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0.99981348390000002</v>
+      </c>
+      <c r="T11">
+        <v>0.99968814939999995</v>
+      </c>
+      <c r="V11" s="4"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12" s="2"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K12" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>0.42</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999949566622537</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0.99960997429999998</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0.99968814939999995</v>
+      </c>
+      <c r="T12">
+        <v>0.99947911690000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13" s="2"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K13" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <v>0.46</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999862905480152</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0.99934825940000005</v>
+      </c>
+      <c r="S13" s="5">
+        <v>0.99947911690000002</v>
+      </c>
+      <c r="T13">
+        <v>0.99913090709999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14" s="2"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K14" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>0.5</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99999627336071584</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0.99891355479999999</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.99913090709999997</v>
+      </c>
+      <c r="T14">
+        <v>0.99855033800000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" s="2"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K15" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L15">
+        <v>13</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <v>0.54</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99998986992028915</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0.99818712129999998</v>
+      </c>
+      <c r="S15" s="5">
+        <v>0.99855033800000004</v>
+      </c>
+      <c r="T15">
+        <v>0.99758298919999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" s="2"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K16" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16">
+        <v>14</v>
+      </c>
+      <c r="N16">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99997246356453784</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0.9969788571</v>
+      </c>
+      <c r="S16" s="5">
+        <v>0.99758298919999999</v>
+      </c>
+      <c r="T16">
+        <v>0.99597042430000005</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" s="2"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K17" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L17">
+        <v>15</v>
+      </c>
+      <c r="M17">
+        <v>15</v>
+      </c>
+      <c r="N17">
+        <v>0.62</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99992514818399925</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0.99496199139999997</v>
+      </c>
+      <c r="S17" s="5">
+        <v>0.99597042430000005</v>
+      </c>
+      <c r="T17">
+        <v>0.99328318439999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18" s="2"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K18" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L18">
+        <v>16</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <v>0.66</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99979653164487448</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0.99160437739999996</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0.99328318439999996</v>
+      </c>
+      <c r="T18">
+        <v>0.98880403520000004</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19" s="2"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="R19" s="5"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K19" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L19">
+        <v>17</v>
+      </c>
+      <c r="M19">
+        <v>17</v>
+      </c>
+      <c r="N19">
+        <v>0.7</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99944691564373245</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0.98600369290000001</v>
+      </c>
+      <c r="S19" s="5">
+        <v>0.98880403520000004</v>
+      </c>
+      <c r="T19">
+        <v>0.9813392393</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20" s="2"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="R20" s="5"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K20" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L20">
+        <v>18</v>
+      </c>
+      <c r="M20">
+        <v>18</v>
+      </c>
+      <c r="N20">
+        <v>0.74</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99849656082088944</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0.97667478569999999</v>
+      </c>
+      <c r="S20" s="5">
+        <v>0.9813392393</v>
+      </c>
+      <c r="T20">
+        <v>0.96889744560000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" s="2"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="R21" s="5"/>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K21" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L21">
+        <v>19</v>
+      </c>
+      <c r="M21">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <v>0.78</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99591322857536713</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0.96112010550000004</v>
+      </c>
+      <c r="S21" s="5">
+        <v>0.96889744560000002</v>
+      </c>
+      <c r="T21">
+        <v>0.94816156579999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" s="2"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="R22" s="5"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K22" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <v>0.82</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.98889100347549141</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0.93520302609999995</v>
+      </c>
+      <c r="S22" s="5">
+        <v>0.94816156579999999</v>
+      </c>
+      <c r="T22">
+        <v>0.9136014093</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23" s="2"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="R23" s="5"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K23" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L23">
+        <v>21</v>
+      </c>
+      <c r="M23">
+        <v>21</v>
+      </c>
+      <c r="N23">
+        <v>0.86</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.96980261659115019</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0.89199979250000005</v>
+      </c>
+      <c r="S23" s="5">
+        <v>0.9136014093</v>
+      </c>
+      <c r="T23">
+        <v>0.85600132470000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24" s="2"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="R24" s="5"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K24" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L24">
+        <v>22</v>
+      </c>
+      <c r="M24">
+        <v>22</v>
+      </c>
+      <c r="N24">
+        <v>0.9</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.91791500138884918</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0.82000285689999997</v>
+      </c>
+      <c r="S24" s="5">
+        <v>0.85600132470000001</v>
+      </c>
+      <c r="T24">
+        <v>0.76000132659999997</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25" s="2"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="R25" s="5"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K25" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L25">
+        <v>23</v>
+      </c>
+      <c r="M25">
+        <v>23</v>
+      </c>
+      <c r="N25">
+        <v>0.94</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="1"/>
+        <v>0.77686983986236013</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0.69999979629999998</v>
+      </c>
+      <c r="S25" s="5">
+        <v>0.76000132659999997</v>
+      </c>
+      <c r="T25">
+        <v>0.60000066969999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26" s="2"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="R26" s="5"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K26" s="5">
+        <v>6.9444444439999999E-4</v>
+      </c>
+      <c r="L26">
+        <v>24</v>
+      </c>
+      <c r="M26">
+        <v>24</v>
+      </c>
+      <c r="N26">
+        <v>0.98</v>
+      </c>
+      <c r="O26" s="2">
+        <f>(((EXP(2.5*N26/0.1) - 1)/(EXP(2.5*1/0.1) - 1)) *-1) +1</f>
+        <v>0.39346934029283109</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0.50000154299999999</v>
+      </c>
+      <c r="S26" s="5">
+        <v>0.60000066969999999</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27" s="2"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="R27" s="5"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" s="2">
+        <f>(((EXP(2.5*N27/0.1) - 1)/(EXP(2.5*1/0.1) - 1)) *-1) +1</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5"/>
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" s="2"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="R28" s="5"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q28" s="5"/>
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" s="2"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="R29" s="5"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q29" s="5"/>
+      <c r="S29" s="5"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30" s="2"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="R30" s="5"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q30" s="5"/>
+      <c r="S30" s="5"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31" s="2"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="R31" s="5"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q31" s="5"/>
+      <c r="S31" s="5"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32" s="2"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="R32" s="5"/>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q32" s="5"/>
+      <c r="S32" s="5"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" s="2"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="R33" s="5"/>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q33" s="5"/>
+      <c r="S33" s="5"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" s="2"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="R34" s="5"/>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q34" s="5"/>
+      <c r="S34" s="5"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35" s="2"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="R35" s="5"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q35" s="5"/>
+      <c r="S35" s="5"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36" s="2"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="R36" s="5"/>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q36" s="5"/>
+      <c r="S36" s="5"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37" s="2"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="R37" s="5"/>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q37" s="5"/>
+      <c r="S37" s="5"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38" s="2"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="R38" s="5"/>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q38" s="5"/>
+      <c r="S38" s="5"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39" s="2"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="R39" s="5"/>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q39" s="5"/>
+      <c r="S39" s="5"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40" s="2"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="R40" s="5"/>
-    </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q40" s="5"/>
+      <c r="S40" s="5"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41" s="2"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="R41" s="5"/>
-    </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q41" s="5"/>
+      <c r="S41" s="5"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
-      <c r="P42" s="5"/>
-    </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
@@ -3407,8 +4311,8 @@
       <c r="B101" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="P3:X42">
-    <sortCondition descending="1" ref="S3:S42"/>
+  <sortState ref="Q3:Y42">
+    <sortCondition descending="1" ref="T3:T42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>